<commit_message>
Final Set Of Data From Azure
</commit_message>
<xml_diff>
--- a/docs/data7repl.xlsx
+++ b/docs/data7repl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USERDATA\chevrotain\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F1DEFE-BBA1-49D2-9B32-31F823465C06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4487892-22BF-4C11-A0A6-55891C35277F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A478AC17-B821-49E0-BBE5-2534ACF29465}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A478AC17-B821-49E0-BBE5-2534ACF29465}"/>
   </bookViews>
   <sheets>
     <sheet name="CvRDT-Y" sheetId="2" r:id="rId1"/>
@@ -1764,7 +1764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DAC9F2-CF17-40D5-B51E-826B3CE40E13}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -2108,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CE1395-6380-422A-83AF-3E7E185B3F85}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H22" sqref="A18:H22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,52 +2137,208 @@
       <c r="O1" s="1"/>
       <c r="S1" s="1"/>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>138.15430000000001</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>141.57634999999999</v>
+      </c>
+      <c r="E2">
+        <v>97.255359999999996</v>
+      </c>
+      <c r="G2">
+        <v>149.01116999999999</v>
+      </c>
+      <c r="H2">
+        <v>97.374700000000004</v>
+      </c>
+      <c r="J2">
+        <v>216.31117</v>
+      </c>
+      <c r="K2">
+        <v>94.033420000000007</v>
+      </c>
+      <c r="M2">
+        <v>544.25744999999995</v>
+      </c>
+      <c r="N2">
+        <v>94.033420000000007</v>
+      </c>
+    </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>136.91359</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>141.46983</v>
+      </c>
+      <c r="E3">
+        <v>97.0167</v>
+      </c>
+      <c r="G3">
+        <v>157.68929</v>
+      </c>
+      <c r="H3">
+        <v>98.090689999999995</v>
+      </c>
+      <c r="J3">
+        <v>219.11931999999999</v>
+      </c>
+      <c r="K3">
+        <v>97.732699999999994</v>
+      </c>
+      <c r="M3">
+        <v>643.39124000000004</v>
+      </c>
+      <c r="N3">
+        <v>95.584723999999994</v>
+      </c>
       <c r="S3" s="2"/>
     </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>137.48409000000001</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>140.36197000000001</v>
+      </c>
+      <c r="E4">
+        <v>97.136039999999994</v>
+      </c>
+      <c r="G4">
+        <v>156.97875999999999</v>
+      </c>
+      <c r="H4">
+        <v>98.090689999999995</v>
+      </c>
+      <c r="J4">
+        <v>287.93221999999997</v>
+      </c>
+      <c r="K4">
+        <v>97.255359999999996</v>
+      </c>
+      <c r="M4">
+        <v>634.18020000000001</v>
+      </c>
+      <c r="N4">
+        <v>87.828156000000007</v>
+      </c>
+    </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>136.80052000000001</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>140.78091000000001</v>
+      </c>
+      <c r="E5">
+        <v>96.658709999999999</v>
+      </c>
+      <c r="G5">
+        <v>149.83242999999999</v>
+      </c>
+      <c r="H5">
+        <v>98.090689999999995</v>
+      </c>
+      <c r="J5">
+        <v>236.29297</v>
+      </c>
+      <c r="K5">
+        <v>92.243440000000007</v>
+      </c>
+      <c r="M5">
+        <v>592.60440000000006</v>
+      </c>
+      <c r="N5">
+        <v>95.107399999999998</v>
+      </c>
       <c r="S5" s="1"/>
     </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>137.57307</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>139.66197</v>
+      </c>
+      <c r="E6">
+        <v>96.778030000000001</v>
+      </c>
+      <c r="G6">
+        <v>148.81301999999999</v>
+      </c>
+      <c r="H6">
+        <v>98.090689999999995</v>
+      </c>
+      <c r="J6">
+        <v>257.21575999999999</v>
+      </c>
+      <c r="K6">
+        <v>96.181389999999993</v>
+      </c>
+      <c r="M6">
+        <v>692.15120000000002</v>
+      </c>
+      <c r="N6">
+        <v>93.317440000000005</v>
+      </c>
+    </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="e">
+      <c r="A7" s="1">
         <f>AVERAGE(A2:A6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B7" s="1" t="e">
+        <v>137.38511400000002</v>
+      </c>
+      <c r="B7" s="1">
         <f>AVERAGE(B2:B6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="1" t="e">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
         <f>AVERAGE(D2:D6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="1" t="e">
+        <v>140.77020599999997</v>
+      </c>
+      <c r="E7" s="1">
         <f>AVERAGE(E2:E6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" s="1" t="e">
+        <v>96.96896799999999</v>
+      </c>
+      <c r="G7" s="1">
         <f>AVERAGE(G2:G6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="1" t="e">
+        <v>152.464934</v>
+      </c>
+      <c r="H7" s="1">
         <f>AVERAGE(H2:H6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" s="1" t="e">
+        <v>97.947491999999997</v>
+      </c>
+      <c r="J7" s="1">
         <f>AVERAGE(J2:J6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K7" s="1" t="e">
+        <v>243.37428799999998</v>
+      </c>
+      <c r="K7" s="1">
         <f>AVERAGE(K2:K6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="1" t="e">
+        <v>95.489262000000011</v>
+      </c>
+      <c r="M7" s="1">
         <f>AVERAGE(M2:M6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N7" s="1" t="e">
+        <v>621.31689800000004</v>
+      </c>
+      <c r="N7" s="1">
         <f>AVERAGE(N2:N6)</f>
-        <v>#DIV/0!</v>
+        <v>93.174227999999999</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -2211,46 +2367,206 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1379.0962</v>
+      </c>
+      <c r="B10">
+        <v>49.284008</v>
+      </c>
+      <c r="D10">
+        <v>1470.3535999999999</v>
+      </c>
+      <c r="E10">
+        <v>64.916466</v>
+      </c>
+      <c r="G10">
+        <v>1635.4519</v>
+      </c>
+      <c r="H10">
+        <v>48.448692000000001</v>
+      </c>
+      <c r="J10">
+        <v>1814.5365999999999</v>
+      </c>
+      <c r="K10">
+        <v>49.164676999999998</v>
+      </c>
+      <c r="M10">
+        <v>1919.6003000000001</v>
+      </c>
+      <c r="N10">
+        <v>47.613365000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1254.6714999999999</v>
+      </c>
+      <c r="B11">
+        <v>48.568019999999997</v>
+      </c>
+      <c r="D11">
+        <v>1377.5020999999999</v>
+      </c>
+      <c r="E11">
+        <v>64.55847</v>
+      </c>
+      <c r="G11">
+        <v>1756.8236999999999</v>
+      </c>
+      <c r="H11">
+        <v>51.193317</v>
+      </c>
+      <c r="J11">
+        <v>1906.9856</v>
+      </c>
+      <c r="K11">
+        <v>42.124104000000003</v>
+      </c>
+      <c r="M11">
+        <v>1878.6364000000001</v>
+      </c>
+      <c r="N11">
+        <v>47.613365000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1249.1376</v>
+      </c>
+      <c r="B12">
+        <v>52.386629999999997</v>
+      </c>
+      <c r="D12">
+        <v>1520.3762999999999</v>
+      </c>
+      <c r="E12">
+        <v>41.408115000000002</v>
+      </c>
+      <c r="G12">
+        <v>1764.0454</v>
+      </c>
+      <c r="H12">
+        <v>46.658720000000002</v>
+      </c>
+      <c r="J12">
+        <v>1875.1229000000001</v>
+      </c>
+      <c r="K12">
+        <v>48.448689999999999</v>
+      </c>
+      <c r="M12">
+        <v>1891.1651999999999</v>
+      </c>
+      <c r="N12">
+        <v>47.136043999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1332.8982000000001</v>
+      </c>
+      <c r="B13">
+        <v>47.732697000000002</v>
+      </c>
+      <c r="D13">
+        <v>1505.4059</v>
+      </c>
+      <c r="E13">
+        <v>56.205249999999999</v>
+      </c>
+      <c r="G13">
+        <v>1680.4880000000001</v>
+      </c>
+      <c r="H13">
+        <v>49.761333</v>
+      </c>
+      <c r="J13">
+        <v>1872.7357999999999</v>
+      </c>
+      <c r="K13">
+        <v>49.403346999999997</v>
+      </c>
+      <c r="M13">
+        <v>1967.0757000000001</v>
+      </c>
+      <c r="N13">
+        <v>47.732697000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1375.9269999999999</v>
+      </c>
+      <c r="B14">
+        <v>51.312649999999998</v>
+      </c>
+      <c r="D14">
+        <v>1449.2662</v>
+      </c>
+      <c r="E14">
+        <v>65.632453999999996</v>
+      </c>
+      <c r="G14">
+        <v>1723.4870000000001</v>
+      </c>
+      <c r="H14">
+        <v>46.658720000000002</v>
+      </c>
+      <c r="J14">
+        <v>2006.7717</v>
+      </c>
+      <c r="K14">
+        <v>53.221960000000003</v>
+      </c>
+      <c r="M14">
+        <v>1867.5138999999999</v>
+      </c>
+      <c r="N14">
+        <v>48.806683</v>
+      </c>
+    </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="e">
+      <c r="A15" s="1">
         <f>AVERAGE(A10:A14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B15" s="1" t="e">
+        <v>1318.3461</v>
+      </c>
+      <c r="B15" s="1">
         <f>AVERAGE(B10:B14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D15" s="1" t="e">
+        <v>49.856800999999997</v>
+      </c>
+      <c r="D15" s="1">
         <f t="shared" ref="D15:E15" si="0">AVERAGE(D10:D14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E15" s="1" t="e">
+        <v>1464.5808199999999</v>
+      </c>
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="1" t="e">
+        <v>58.544151000000014</v>
+      </c>
+      <c r="G15" s="1">
         <f>AVERAGE(G10:G14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="1" t="e">
+        <v>1712.0592000000001</v>
+      </c>
+      <c r="H15" s="1">
         <f>AVERAGE(H10:H14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="1" t="e">
+        <v>48.544156399999999</v>
+      </c>
+      <c r="J15" s="1">
         <f>AVERAGE(J10:J14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="1" t="e">
+        <v>1895.2305199999998</v>
+      </c>
+      <c r="K15" s="1">
         <f>AVERAGE(K10:K14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" s="1" t="e">
+        <v>48.4725556</v>
+      </c>
+      <c r="M15" s="1">
         <f>AVERAGE(M10:M14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N15" s="1" t="e">
+        <v>1904.7982999999999</v>
+      </c>
+      <c r="N15" s="1">
         <f>AVERAGE(N10:N14)</f>
-        <v>#DIV/0!</v>
+        <v>47.780430799999998</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -2272,52 +2588,142 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1962.2244000000001</v>
+      </c>
+      <c r="B18">
+        <v>52.625298000000001</v>
+      </c>
+      <c r="D18">
+        <v>1903.2737</v>
+      </c>
+      <c r="E18">
+        <v>52.505961999999997</v>
+      </c>
+      <c r="G18">
+        <v>1957.1813</v>
+      </c>
+      <c r="H18">
+        <v>52.267299999999999</v>
+      </c>
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1992.4329</v>
+      </c>
+      <c r="B19">
+        <v>48.926014000000002</v>
+      </c>
+      <c r="D19">
+        <v>1933.1799000000001</v>
+      </c>
+      <c r="E19">
+        <v>47.971355000000003</v>
+      </c>
+      <c r="G19">
+        <v>1983.0354</v>
+      </c>
+      <c r="H19">
+        <v>49.522675</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1915.9952000000001</v>
+      </c>
+      <c r="B20">
+        <v>49.642006000000002</v>
+      </c>
+      <c r="D20">
+        <v>1892.4719</v>
+      </c>
+      <c r="E20">
+        <v>49.045344999999998</v>
+      </c>
+      <c r="G20">
+        <v>1907.6596999999999</v>
+      </c>
+      <c r="H20">
+        <v>50.835323000000002</v>
+      </c>
       <c r="N20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1896.6304</v>
+      </c>
+      <c r="B21">
+        <v>47.613365000000002</v>
+      </c>
+      <c r="D21">
+        <v>1889.6527000000001</v>
+      </c>
+      <c r="E21">
+        <v>46.897373000000002</v>
+      </c>
+      <c r="G21">
+        <v>1922.0762999999999</v>
+      </c>
+      <c r="H21">
+        <v>45.226726999999997</v>
+      </c>
       <c r="N21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1928.9751000000001</v>
+      </c>
+      <c r="B22">
+        <v>54.415275999999999</v>
+      </c>
+      <c r="D22">
+        <v>1955.5446999999999</v>
+      </c>
+      <c r="E22">
+        <v>48.687350000000002</v>
+      </c>
+      <c r="G22">
+        <v>1928.6741999999999</v>
+      </c>
+      <c r="H22">
+        <v>55.608592999999999</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="e">
+      <c r="A23" s="1">
         <f>AVERAGE(A18:A22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B23" s="1" t="e">
+        <v>1939.2516000000001</v>
+      </c>
+      <c r="B23" s="1">
         <f>AVERAGE(B18:B22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" s="1" t="e">
+        <v>50.644391800000008</v>
+      </c>
+      <c r="D23" s="1">
         <f t="shared" ref="D23:E23" si="1">AVERAGE(D18:D22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="1" t="e">
+        <v>1914.82458</v>
+      </c>
+      <c r="E23" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G23" s="1" t="e">
+        <v>49.021476999999997</v>
+      </c>
+      <c r="G23" s="1">
         <f t="shared" ref="G23:H23" si="2">AVERAGE(G18:G22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H23" s="1" t="e">
+        <v>1939.7253799999999</v>
+      </c>
+      <c r="H23" s="1">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>50.692123599999988</v>
       </c>
       <c r="L23" s="1"/>
       <c r="N23" s="1"/>

</xml_diff>